<commit_message>
password reset basics working
</commit_message>
<xml_diff>
--- a/details/worktimes.xlsx
+++ b/details/worktimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files (x86)\Programming\VS code\Bet servus\details\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E899C45-6EDC-4F8D-839F-40CA69327073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853A23D4-3459-40D6-8569-9EAD38AC4BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36846866-D087-4854-A8AB-FEDE182B4FBC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Projekt rész</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>regisztráció backend/titkosítás</t>
+  </si>
+  <si>
+    <t>elfelejtett jelszó backend</t>
+  </si>
+  <si>
+    <t>elfelejtett jelszó frontend</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47AE056-6196-4814-B5F2-D4174231B88D}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -532,7 +538,7 @@
       </c>
       <c r="H3" s="5">
         <f ca="1">SUMIF(B:C,G3,$C$1)+SUMIF(B:C,$B$3,$C$1)</f>
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -550,7 +556,7 @@
       </c>
       <c r="H4" s="5">
         <f t="shared" ref="H4:H6" ca="1" si="0">SUMIF(B:C,G4,$C$1)+SUMIF(B:C,$B$3,$C$1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -594,7 +600,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -608,6 +614,28 @@
         <v>4</v>
       </c>
       <c r="C8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>